<commit_message>
Add debug option and change comments to not be ass
- Introduced a Debug variable to enable debug messages, updated settings management to include Debug, and refactored code for clarity and maintainability.

- Impedance calculation and CLI dialogs now support debug output.

- Updated Excel settings and data files to support the new Debug option.

- Updated all comment (more detail in the functions)
</commit_message>
<xml_diff>
--- a/MSO5000 LCR/Data/Clean.xlsx
+++ b/MSO5000 LCR/Data/Clean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonz\source\repos\MSO5000 LCR\MSO5000 LCR\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonz\source\repos\MSO5000-LCR-meter\MSO5000 LCR\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2F1A8C-15B4-4E4E-823E-63F734663204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8F6C88-7854-430A-A3CC-2EF9CC6AEAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="2800" windowWidth="16800" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>F  [Hz]</t>
   </si>
   <si>
-    <t>I [mA]</t>
-  </si>
-  <si>
     <r>
       <t>Z (abs) [</t>
     </r>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>X [Ω]</t>
+  </si>
+  <si>
+    <t>I [A]</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -464,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -473,16 +473,16 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>0.2512480738027979</v>
+        <v>2.5124807380279789E-4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>0.50202101681830102</v>
+        <v>5.0202101681830105E-4</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -520,7 +520,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>0.75184817764144152</v>
+        <v>7.5184817764144154E-4</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>1.0002677655055627</v>
+        <v>1.0002677655055628E-3</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -550,7 +550,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>1.2468310391348656</v>
+        <v>1.2468310391348656E-3</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -565,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>1.4911062163765088</v>
+        <v>1.4911062163765088E-3</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -580,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>1.732682028419033</v>
+        <v>1.7326820284190329E-3</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -595,7 +595,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>1.971170855562723</v>
+        <v>1.9711708555627231E-3</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -610,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>2.2062113964520109</v>
+        <v>2.206211396452011E-3</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -625,7 +625,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="2">
-        <v>2.4374708385970858</v>
+        <v>2.4374708385970856E-3</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2">
-        <v>4.491102074175144</v>
+        <v>4.4911020741751437E-3</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -655,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>6.0203306759153445</v>
+        <v>6.0203306759153445E-3</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>7.0897656983829247</v>
+        <v>7.0897656983829249E-3</v>
       </c>
       <c r="C14">
         <v>40</v>
@@ -685,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2">
-        <v>7.8247898582699866</v>
+        <v>7.8247898582699867E-3</v>
       </c>
       <c r="C15">
         <v>50</v>
@@ -700,7 +700,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="2">
-        <v>8.3340218394238761</v>
+        <v>8.3340218394238764E-3</v>
       </c>
       <c r="C16">
         <v>60</v>
@@ -715,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="2">
-        <v>8.6937114773202406</v>
+        <v>8.6937114773202404E-3</v>
       </c>
       <c r="C17">
         <v>70</v>
@@ -730,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>8.9537099005424352</v>
+        <v>8.9537099005424347E-3</v>
       </c>
       <c r="C18">
         <v>80</v>
@@ -745,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>9.1460658855750001</v>
+        <v>9.1460658855750006E-3</v>
       </c>
       <c r="C19">
         <v>90</v>
@@ -760,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>9.2915203357813887</v>
+        <v>9.2915203357813881E-3</v>
       </c>
       <c r="C20">
         <v>100</v>

</xml_diff>

<commit_message>
Update VS workspace and data files
Updated Visual Studio workspace layout and index files, modified several Excel data files, and made changes to Calculation.py and Misc.py. These changes improve project organization and update supporting data and code for ongoing development.
</commit_message>
<xml_diff>
--- a/MSO5000 LCR/Data/Clean.xlsx
+++ b/MSO5000 LCR/Data/Clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonz\source\repos\MSO5000-LCR-meter\MSO5000 LCR\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771A1645-467B-4A76-9B80-1FEE2EE08B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01EDED6-E734-4E66-AABA-13A76EF259C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3610" windowWidth="16800" windowHeight="9670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>U_[V]</t>
-  </si>
-  <si>
-    <t>I_[A]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>F_[Hz]</t>
   </si>
@@ -57,6 +51,21 @@
   </si>
   <si>
     <t>X_[Ω]</t>
+  </si>
+  <si>
+    <t>Ue_[V]</t>
+  </si>
+  <si>
+    <t>Ua_[V]</t>
+  </si>
+  <si>
+    <t>Ie_[A]</t>
+  </si>
+  <si>
+    <t>H_[1]</t>
+  </si>
+  <si>
+    <t>H_[db]</t>
   </si>
 </sst>
 </file>
@@ -420,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H201"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,2829 +440,3438 @@
     <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2" s="2">
+        <v>4.9999013068781659</v>
+      </c>
+      <c r="C2" s="2">
         <v>3.14153064287249E-5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-89.6400047372979</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3" s="2">
+        <v>4.9975344238193102</v>
+      </c>
+      <c r="C3" s="2">
         <v>1.5700217431932842E-4</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
       <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
         <v>-88.200591825838373</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4" s="2">
+        <v>4.9901595225182245</v>
+      </c>
+      <c r="C4" s="2">
         <v>3.1354096992368803E-4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-86.404726220131835</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" s="2">
+        <v>4.9779402435160094</v>
+      </c>
+      <c r="C5" s="2">
         <v>4.6915981497116637E-4</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-84.615904082606434</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2">
+        <v>4.9609830769679579</v>
+      </c>
+      <c r="C6" s="2">
         <v>6.234155195674328E-4</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>20</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-82.837544193274184</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="2">
+        <v>4.9394335096009065</v>
+      </c>
+      <c r="C7" s="2">
         <v>7.7588440133287276E-4</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>25</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-81.072945131040072</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" s="2">
+        <v>4.9134726274500142</v>
+      </c>
+      <c r="C8" s="2">
         <v>9.2616777060069012E-4</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>-79.325250587631245</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" s="2">
+        <v>4.8833130194900374</v>
+      </c>
+      <c r="C9" s="2">
         <v>1.0738966215046504E-3</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>35</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>-77.597418926878589</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" s="2">
+        <v>4.8491941575634199</v>
+      </c>
+      <c r="C10" s="2">
         <v>1.2187354192985428E-3</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>40</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>-75.892197628409875</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11" s="2">
+        <v>4.811377439480947</v>
+      </c>
+      <c r="C11" s="2">
         <v>1.360384921576891E-3</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>45</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>-74.212103024879184</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" s="2">
+        <v>4.7701410818923247</v>
+      </c>
+      <c r="C12" s="2">
         <v>1.4985840179459796E-3</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>50</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>-72.55940550948813</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" s="2">
+        <v>4.7257750386995774</v>
+      </c>
+      <c r="C13" s="2">
         <v>1.6331106158506273E-3</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>55</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>-70.936120170854721</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14" s="2">
+        <v>4.6785761013935243</v>
+      </c>
+      <c r="C14" s="2">
         <v>1.7637816371278406E-3</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>60</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>-69.344002617660351</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5</v>
       </c>
       <c r="B15" s="2">
+        <v>4.6288433121747268</v>
+      </c>
+      <c r="C15" s="2">
         <v>1.8904522187390275E-3</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>65</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>-67.784549594839405</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16" s="2">
+        <v>4.5768737916637061</v>
+      </c>
+      <c r="C16" s="2">
         <v>2.0130142312417706E-3</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>70</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>-66.259003871443738</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17" s="2">
+        <v>4.5229590528681545</v>
+      </c>
+      <c r="C17" s="2">
         <v>2.1313942399467066E-3</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>75</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-64.768362799132177</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" s="2">
+        <v>4.4673818439702391</v>
+      </c>
+      <c r="C18" s="2">
         <v>2.2455510370875719E-3</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>80</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>-63.313389897784695</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" s="2">
+        <v>4.4104135360648149</v>
+      </c>
+      <c r="C19" s="2">
         <v>2.3554728699130144E-3</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>85</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>-61.89462881689834</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5</v>
       </c>
       <c r="B20" s="2">
+        <v>4.3523120493339258</v>
+      </c>
+      <c r="C20" s="2">
         <v>2.4611744808572034E-3</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>90</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>-60.512419042487068</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21" s="2">
+        <v>4.2933202928902547</v>
+      </c>
+      <c r="C21" s="2">
         <v>2.5626940634138804E-3</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>95</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>-59.166912762694949</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22" s="2">
+        <v>4.2336650798241529</v>
+      </c>
+      <c r="C22" s="2">
         <v>2.6600902225070405E-3</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>100</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>-57.858092364657949</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5</v>
       </c>
       <c r="B23" s="2">
+        <v>4.173556469655102</v>
+      </c>
+      <c r="C23" s="2">
         <v>2.7534390123262302E-3</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>105</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>-56.585788104156315</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5</v>
       </c>
       <c r="B24" s="2">
+        <v>4.1131874849798002</v>
+      </c>
+      <c r="C24" s="2">
         <v>2.8428311088430046E-3</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>110</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>-55.34969556291724</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5</v>
       </c>
       <c r="B25" s="2">
+        <v>4.0527341470351343</v>
+      </c>
+      <c r="C25" s="2">
         <v>2.9283691593539572E-3</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>115</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>-54.149392581664344</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5</v>
       </c>
       <c r="B26" s="2">
+        <v>3.9923557754987438</v>
+      </c>
+      <c r="C26" s="2">
         <v>3.0101653379576722E-3</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>120</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>-52.984355426817935</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>5</v>
       </c>
       <c r="B27" s="2">
+        <v>3.9321955004769165</v>
+      </c>
+      <c r="C27" s="2">
         <v>3.0883391241942801E-3</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>125</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>-51.853974012777456</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28" s="2">
+        <v>3.87238093867099</v>
+      </c>
+      <c r="C28" s="2">
         <v>3.1630153122957816E-3</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>130</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>-50.757566058507848</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29" s="2">
+        <v>3.8130249906381315</v>
+      </c>
+      <c r="C29" s="2">
         <v>3.2343222506066214E-3</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>135</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>-49.694390105989861</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30" s="2">
+        <v>3.7542267214302956</v>
+      </c>
+      <c r="C30" s="2">
         <v>3.3023903046276552E-3</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>140</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>-48.663657368854381</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5</v>
       </c>
       <c r="B31" s="2">
+        <v>3.6960722923601819</v>
+      </c>
+      <c r="C31" s="2">
         <v>3.3673505326365046E-3</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>145</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>-47.664542412504048</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32" s="2">
+        <v>3.6386359169476363</v>
+      </c>
+      <c r="C32" s="2">
         <v>3.4293335597311964E-3</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>150</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>-46.696192692829342</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33" s="2">
+        <v>3.5819808190653197</v>
+      </c>
+      <c r="C33" s="2">
         <v>3.4884686342072989E-3</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>155</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>-45.757737000022317</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5</v>
       </c>
       <c r="B34" s="2">
+        <v>3.5261601758156447</v>
+      </c>
+      <c r="C34" s="2">
         <v>3.5448828491914624E-3</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>160</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>-44.848292867834715</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>5</v>
       </c>
       <c r="B35" s="2">
+        <v>3.4712180316720036</v>
+      </c>
+      <c r="C35" s="2">
         <v>3.5987005122120317E-3</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>165</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>-43.966973017788824</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" s="2">
+        <v>3.4171901738867652</v>
+      </c>
+      <c r="C36" s="2">
         <v>3.650042645708642E-3</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>170</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>-43.112890913164243</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>5</v>
       </c>
       <c r="B37" s="2">
+        <v>3.3641049621161208</v>
+      </c>
+      <c r="C37" s="2">
         <v>3.6990266022111406E-3</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>175</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>-42.285165499819598</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
       <c r="B38" s="2">
+        <v>3.3119841076676995</v>
+      </c>
+      <c r="C38" s="2">
         <v>3.7457657789237964E-3</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>180</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>-41.482925210750736</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>5</v>
       </c>
       <c r="B39" s="2">
+        <v>3.2608433997831003</v>
+      </c>
+      <c r="C39" s="2">
         <v>3.7903694176281799E-3</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>185</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>-40.705311309328266</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>5</v>
       </c>
       <c r="B40" s="2">
+        <v>3.210693377973175</v>
+      </c>
+      <c r="C40" s="2">
         <v>3.8329424770845708E-3</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>190</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>-39.951480642896946</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>5</v>
       </c>
       <c r="B41" s="2">
+        <v>3.1615399506801061</v>
+      </c>
+      <c r="C41" s="2">
         <v>3.8735855664040302E-3</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>195</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>-39.220607874272226</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
       <c r="B42" s="2">
+        <v>3.1133849614974989</v>
+      </c>
+      <c r="C42" s="2">
         <v>3.9123949291349934E-3</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>200</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>-38.511887253966584</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>5</v>
       </c>
       <c r="B43" s="2">
+        <v>3.0662267048852669</v>
+      </c>
+      <c r="C43" s="2">
         <v>3.9494624690264409E-3</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>205</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>-37.824533990984968</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>5</v>
       </c>
       <c r="B44" s="2">
+        <v>3.0200603938135169</v>
+      </c>
+      <c r="C44" s="2">
         <v>3.9848758095728581E-3</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>210</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>-37.157785274945311</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>5</v>
       </c>
       <c r="B45" s="2">
+        <v>2.9748785820976433</v>
+      </c>
+      <c r="C45" s="2">
         <v>4.0187183805010171E-3</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>215</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>-36.510900997260094</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>5</v>
       </c>
       <c r="B46" s="2">
+        <v>2.9306715443791651</v>
+      </c>
+      <c r="C46" s="2">
         <v>4.0510695253187451E-3</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>220</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>-35.883164214265733</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>5</v>
       </c>
       <c r="B47" s="2">
+        <v>2.8874276167926203</v>
+      </c>
+      <c r="C47" s="2">
         <v>4.0820046249095913E-3</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>225</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>-35.273881390585245</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>5</v>
       </c>
       <c r="B48" s="2">
+        <v>2.8451335013624011</v>
+      </c>
+      <c r="C48" s="2">
         <v>4.1115952329266701E-3</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>230</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>-34.682382456702889</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>5</v>
       </c>
       <c r="B49" s="2">
+        <v>2.8037745371153653</v>
+      </c>
+      <c r="C49" s="2">
         <v>4.1399092194181648E-3</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>235</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>-34.108020710746359</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>5</v>
       </c>
       <c r="B50" s="2">
+        <v>2.7633349407919168</v>
+      </c>
+      <c r="C50" s="2">
         <v>4.1670109197119382E-3</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>240</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>-33.550172590822328</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>5</v>
       </c>
       <c r="B51" s="2">
+        <v>2.7237980199037848</v>
+      </c>
+      <c r="C51" s="2">
         <v>4.1929612861041562E-3</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>245</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>-33.008237340935523</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>5</v>
       </c>
       <c r="B52" s="2">
+        <v>2.6851463607315758</v>
+      </c>
+      <c r="C52" s="2">
         <v>4.2178180403438428E-3</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>250</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>-32.481636590529753</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>5</v>
       </c>
       <c r="B53" s="2">
+        <v>2.6473619936879937</v>
+      </c>
+      <c r="C53" s="2">
         <v>4.2416358252891457E-3</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>255</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>-31.969813865008028</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>5</v>
       </c>
       <c r="B54" s="2">
+        <v>2.6104265382999499</v>
+      </c>
+      <c r="C54" s="2">
         <v>4.2644663544386579E-3</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>260</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>-31.472234042197247</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>5</v>
       </c>
       <c r="B55" s="2">
+        <v>2.5743213298895768</v>
+      </c>
+      <c r="C55" s="2">
         <v>4.2863585583191189E-3</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>265</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>-30.988382767602364</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>5</v>
       </c>
       <c r="B56" s="2">
+        <v>2.5390275298642595</v>
+      </c>
+      <c r="C56" s="2">
         <v>4.3073587269452495E-3</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>270</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>-30.517765839421301</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>5</v>
       </c>
       <c r="B57" s="2">
+        <v>2.5045262213616981</v>
+      </c>
+      <c r="C57" s="2">
         <v>4.3275106477641033E-3</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>275</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>-30.059908572644037</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>5</v>
       </c>
       <c r="B58" s="2">
+        <v>2.4707984918397505</v>
+      </c>
+      <c r="C58" s="2">
         <v>4.3468557386601202E-3</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>280</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>-29.614355150116502</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>5</v>
       </c>
       <c r="B59" s="2">
+        <v>2.4378255040533316</v>
+      </c>
+      <c r="C59" s="2">
         <v>4.3654331757326352E-3</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>285</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>-29.180667967188818</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>5</v>
       </c>
       <c r="B60" s="2">
+        <v>2.4055885567229316</v>
+      </c>
+      <c r="C60" s="2">
         <v>4.3832800156690518E-3</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>290</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>-28.758426975471835</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>5</v>
       </c>
       <c r="B61" s="2">
+        <v>2.3740691360713266</v>
+      </c>
+      <c r="C61" s="2">
         <v>4.4004313126276094E-3</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>295</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>-28.347229030275219</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>5</v>
       </c>
       <c r="B62" s="2">
+        <v>2.3432489592871146</v>
+      </c>
+      <c r="C62" s="2">
         <v>4.416920229616996E-3</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>300</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>-27.946687245478877</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
       <c r="B63" s="2">
+        <v>2.3131100108653375</v>
+      </c>
+      <c r="C63" s="2">
         <v>4.4327781444185267E-3</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>305</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>-27.556430358882025</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>5</v>
       </c>
       <c r="B64" s="2">
+        <v>2.2836345726765304</v>
+      </c>
+      <c r="C64" s="2">
         <v>4.4480347501426381E-3</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>310</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>-27.176102110467237</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>5</v>
       </c>
       <c r="B65" s="2">
+        <v>2.2548052485253676</v>
+      </c>
+      <c r="C65" s="2">
         <v>4.4627181505470914E-3</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>315</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>-26.805360635496761</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>5</v>
       </c>
       <c r="B66" s="2">
+        <v>2.2266049838783926</v>
+      </c>
+      <c r="C66" s="2">
         <v>4.4768549502712173E-3</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>320</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>-26.443877873916215</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>5</v>
       </c>
       <c r="B67" s="2">
+        <v>2.1990170813663172</v>
+      </c>
+      <c r="C67" s="2">
         <v>4.4904703401602783E-3</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>325</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>-26.091338997164481</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>5</v>
       </c>
       <c r="B68" s="2">
+        <v>2.1720252125996811</v>
+      </c>
+      <c r="C68" s="2">
         <v>4.5035881778678778E-3</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>330</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>-25.747441853171068</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>5</v>
       </c>
       <c r="B69" s="2">
+        <v>2.1456134267765781</v>
+      </c>
+      <c r="C69" s="2">
         <v>4.516231063933296E-3</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>335</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>-25.411896430054835</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>5</v>
       </c>
       <c r="B70" s="2">
+        <v>2.1197661565072021</v>
+      </c>
+      <c r="C70" s="2">
         <v>4.5284204135356831E-3</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>340</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>-25.084424338814248</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>5</v>
       </c>
       <c r="B71" s="2">
+        <v>2.0944682212315713</v>
+      </c>
+      <c r="C71" s="2">
         <v>4.5401765241288861E-3</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>345</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>-24.764758315113202</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>5</v>
       </c>
       <c r="B72" s="2">
+        <v>2.0697048285634674</v>
+      </c>
+      <c r="C72" s="2">
         <v>4.5515186391600175E-3</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <v>350</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>-24.452641740112796</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>5</v>
       </c>
       <c r="B73" s="2">
+        <v>2.0454615738549031</v>
+      </c>
+      <c r="C73" s="2">
         <v>4.5624650080721739E-3</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <v>355</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>-24.147828180173331</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>5</v>
       </c>
       <c r="B74" s="2">
+        <v>2.0217244382408541</v>
+      </c>
+      <c r="C74" s="2">
         <v>4.5730329427875003E-3</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <v>360</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>-23.850080945149021</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>5</v>
       </c>
       <c r="B75" s="2">
+        <v>1.9984797853931733</v>
+      </c>
+      <c r="C75" s="2">
         <v>4.5832388708613968E-3</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <v>365</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>-23.5591726649157</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>5</v>
       </c>
       <c r="B76" s="2">
+        <v>1.9757143571851652</v>
+      </c>
+      <c r="C76" s="2">
         <v>4.5930983854923484E-3</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <v>370</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>-23.274884883707784</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>5</v>
       </c>
       <c r="B77" s="2">
+        <v>1.9534152684438428</v>
+      </c>
+      <c r="C77" s="2">
         <v>4.6026262925649829E-3</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <v>375</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>-22.997007671790534</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>5</v>
       </c>
       <c r="B78" s="2">
+        <v>1.9315700009452481</v>
+      </c>
+      <c r="C78" s="2">
         <v>4.6118366548966562E-3</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <v>380</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>-22.725339253956722</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>5</v>
       </c>
       <c r="B79" s="2">
+        <v>1.9101663967888878</v>
+      </c>
+      <c r="C79" s="2">
         <v>4.6207428338502629E-3</v>
       </c>
-      <c r="C79">
+      <c r="D79">
         <v>385</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>-22.45968565430973</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>5</v>
       </c>
       <c r="B80" s="2">
+        <v>1.8891926512702901</v>
+      </c>
+      <c r="C80" s="2">
         <v>4.6293575284683218E-3</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <v>390</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>-22.199860356777002</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>5</v>
       </c>
       <c r="B81" s="2">
+        <v>1.8686373053555203</v>
+      </c>
+      <c r="C81" s="2">
         <v>4.637692812275696E-3</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <v>395</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>-21.945683980787255</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>5</v>
       </c>
       <c r="B82" s="2">
+        <v>1.8484892378480942</v>
+      </c>
+      <c r="C82" s="2">
         <v>4.645760167890694E-3</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <v>400</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>-21.696983971540057</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>5</v>
       </c>
       <c r="B83" s="2">
+        <v>1.828737657326851</v>
+      </c>
+      <c r="C83" s="2">
         <v>4.6535705195768443E-3</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <v>405</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>-21.45359430429675</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>5</v>
       </c>
       <c r="B84" s="2">
+        <v>1.809372093922879</v>
+      </c>
+      <c r="C84" s="2">
         <v>4.6611342638603675E-3</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>410</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>-21.2153552021264</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>5</v>
       </c>
       <c r="B85" s="2">
+        <v>1.7903823909943117</v>
+      </c>
+      <c r="C85" s="2">
         <v>4.6684612983313341E-3</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <v>415</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>-20.982112866548093</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>5</v>
       </c>
       <c r="B86" s="2">
+        <v>1.7717586967496461</v>
+      </c>
+      <c r="C86" s="2">
         <v>4.6755610487397119E-3</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <v>420</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>-20.753719220521525</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>5</v>
       </c>
       <c r="B87" s="2">
+        <v>1.7534914558630388</v>
+      </c>
+      <c r="C87" s="2">
         <v>4.682442494491023E-3</v>
       </c>
-      <c r="C87">
+      <c r="D87">
         <v>425</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>-20.530031663250362</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>5</v>
       </c>
       <c r="B88" s="2">
+        <v>1.7355714011186874</v>
+      </c>
+      <c r="C88" s="2">
         <v>4.6891141926401108E-3</v>
       </c>
-      <c r="C88">
+      <c r="D88">
         <v>430</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>-20.310912836277232</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>5</v>
       </c>
       <c r="B89" s="2">
+        <v>1.7179895451158333</v>
+      </c>
+      <c r="C89" s="2">
         <v>4.695584300475575E-3</v>
       </c>
-      <c r="C89">
+      <c r="D89">
         <v>435</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>-20.096230400364533</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>5</v>
       </c>
       <c r="B90" s="2">
+        <v>1.7007371720610067</v>
+      </c>
+      <c r="C90" s="2">
         <v>4.7018605967818674E-3</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <v>440</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>-19.885856822671617</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>5</v>
       </c>
       <c r="B91" s="2">
+        <v>1.6838058296698635</v>
+      </c>
+      <c r="C91" s="2">
         <v>4.7079505018606327E-3</v>
       </c>
-      <c r="C91">
+      <c r="D91">
         <v>445</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>-19.679669173755936</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>5</v>
       </c>
       <c r="B92" s="2">
+        <v>1.6671873211971509</v>
+      </c>
+      <c r="C92" s="2">
         <v>4.7138610963879148E-3</v>
       </c>
-      <c r="C92">
+      <c r="D92">
         <v>450</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>-19.477548933942966</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>5</v>
       </c>
       <c r="B93" s="2">
+        <v>1.6508736976100931</v>
+      </c>
+      <c r="C93" s="2">
         <v>4.7195991391790022E-3</v>
       </c>
-      <c r="C93">
+      <c r="D93">
         <v>455</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>-19.279381808627285</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>5</v>
       </c>
       <c r="B94" s="2">
+        <v>1.6348572499175558</v>
+      </c>
+      <c r="C94" s="2">
         <v>4.7251710839282856E-3</v>
       </c>
-      <c r="C94">
+      <c r="D94">
         <v>460</v>
       </c>
-      <c r="D94">
+      <c r="E94">
         <v>-19.085057552084535</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>5</v>
       </c>
       <c r="B95" s="2">
+        <v>1.6191305016648736</v>
+      </c>
+      <c r="C95" s="2">
         <v>4.7305830949871761E-3</v>
       </c>
-      <c r="C95">
+      <c r="D95">
         <v>465</v>
       </c>
-      <c r="D95">
+      <c r="E95">
         <v>-18.894469799391498</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>5</v>
       </c>
       <c r="B96" s="2">
+        <v>1.6036862016020159</v>
+      </c>
+      <c r="C96" s="2">
         <v>4.7358410622392409E-3</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>470</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>-18.707515906068522</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>5</v>
       </c>
       <c r="B97" s="2">
+        <v>1.5885173165308757</v>
+      </c>
+      <c r="C97" s="2">
         <v>4.7409506151278921E-3</v>
       </c>
-      <c r="C97">
+      <c r="D97">
         <v>475</v>
       </c>
-      <c r="D97">
+      <c r="E97">
         <v>-18.52409679507549</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>5</v>
       </c>
       <c r="B98" s="2">
+        <v>1.5736170243358161</v>
+      </c>
+      <c r="C98" s="2">
         <v>4.7459171358885405E-3</v>
       </c>
-      <c r="C98">
+      <c r="D98">
         <v>480</v>
       </c>
-      <c r="D98">
+      <c r="E98">
         <v>-18.344116810808607</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>5</v>
       </c>
       <c r="B99" s="2">
+        <v>1.5589787072001895</v>
+      </c>
+      <c r="C99" s="2">
         <v>4.7507457720337371E-3</v>
       </c>
-      <c r="C99">
+      <c r="D99">
         <v>485</v>
       </c>
-      <c r="D99">
+      <c r="E99">
         <v>-18.167483579761765</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>5</v>
       </c>
       <c r="B100" s="2">
+        <v>1.5445959450103206</v>
+      </c>
+      <c r="C100" s="2">
         <v>4.7554414481368263E-3</v>
       </c>
-      <c r="C100">
+      <c r="D100">
         <v>490</v>
       </c>
-      <c r="D100">
+      <c r="E100">
         <v>-17.99410787753116</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>5</v>
       </c>
       <c r="B101" s="2">
+        <v>1.5304625089473902</v>
+      </c>
+      <c r="C101" s="2">
         <v>4.7600088769566874E-3</v>
       </c>
-      <c r="C101">
+      <c r="D101">
         <v>495</v>
       </c>
-      <c r="D101">
+      <c r="E101">
         <v>-17.823903501857334</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>5</v>
       </c>
       <c r="B102" s="2">
+        <v>1.5165723552667643</v>
+      </c>
+      <c r="C102" s="2">
         <v>4.7644525699434359E-3</v>
       </c>
-      <c r="C102">
+      <c r="D102">
         <v>500</v>
       </c>
-      <c r="D102">
+      <c r="E102">
         <v>-17.65678715141286</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>5</v>
       </c>
       <c r="B103" s="2">
+        <v>1.5029196192635432</v>
+      </c>
+      <c r="C103" s="2">
         <v>4.7687768471624589E-3</v>
       </c>
-      <c r="C103">
+      <c r="D103">
         <v>505</v>
       </c>
-      <c r="D103">
+      <c r="E103">
         <v>-17.492678310058114</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>5</v>
       </c>
       <c r="B104" s="2">
+        <v>1.4894986094224687</v>
+      </c>
+      <c r="C104" s="2">
         <v>4.7729858466717175E-3</v>
       </c>
-      <c r="C104">
+      <c r="D104">
         <v>510</v>
       </c>
-      <c r="D104">
+      <c r="E104">
         <v>-17.331499136300739</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>5</v>
       </c>
       <c r="B105" s="2">
+        <v>1.4763038017497809</v>
+      </c>
+      <c r="C105" s="2">
         <v>4.7770835333851075E-3</v>
       </c>
-      <c r="C105">
+      <c r="D105">
         <v>515</v>
       </c>
-      <c r="D105">
+      <c r="E105">
         <v>-17.173174357707389</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>5</v>
       </c>
       <c r="B106" s="2">
+        <v>1.4633298342841627</v>
+      </c>
+      <c r="C106" s="2">
         <v>4.78107370745253E-3</v>
       </c>
-      <c r="C106">
+      <c r="D106">
         <v>520</v>
       </c>
-      <c r="D106">
+      <c r="E106">
         <v>-17.017631170028444</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>5</v>
       </c>
       <c r="B107" s="2">
+        <v>1.4505715017835508</v>
+      </c>
+      <c r="C107" s="2">
         <v>4.784960012185412E-3</v>
       </c>
-      <c r="C107">
+      <c r="D107">
         <v>525</v>
       </c>
-      <c r="D107">
+      <c r="E107">
         <v>-16.864799140808408</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>5</v>
       </c>
       <c r="B108" s="2">
+        <v>1.4380237505842741</v>
+      </c>
+      <c r="C108" s="2">
         <v>4.7887459415545883E-3</v>
       </c>
-      <c r="C108">
+      <c r="D108">
         <v>530</v>
       </c>
-      <c r="D108">
+      <c r="E108">
         <v>-16.714610117265625</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>5</v>
       </c>
       <c r="B109" s="2">
+        <v>1.425681673628757</v>
+      </c>
+      <c r="C109" s="2">
         <v>4.7924348472857831E-3</v>
       </c>
-      <c r="C109">
+      <c r="D109">
         <v>535</v>
       </c>
-      <c r="D109">
+      <c r="E109">
         <v>-16.566998138235945</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>5</v>
       </c>
       <c r="B110" s="2">
+        <v>1.4135405056578194</v>
+      </c>
+      <c r="C110" s="2">
         <v>4.7960299455763033E-3</v>
       </c>
-      <c r="C110">
+      <c r="D110">
         <v>540</v>
       </c>
-      <c r="D110">
+      <c r="E110">
         <v>-16.421899349984972</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>5</v>
       </c>
       <c r="B111" s="2">
+        <v>1.4015956185634786</v>
+      </c>
+      <c r="C111" s="2">
         <v>4.7995343234551058E-3</v>
       </c>
-      <c r="C111">
+      <c r="D111">
         <v>545</v>
       </c>
-      <c r="D111">
+      <c r="E111">
         <v>-16.279251925703477</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>5</v>
       </c>
       <c r="B112" s="2">
+        <v>1.3898425168980435</v>
+      </c>
+      <c r="C112" s="2">
         <v>4.8029509448070063E-3</v>
       </c>
-      <c r="C112">
+      <c r="D112">
         <v>550</v>
       </c>
-      <c r="D112">
+      <c r="E112">
         <v>-16.138995988509603</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>5</v>
       </c>
       <c r="B113" s="2">
+        <v>1.3782768335352316</v>
+      </c>
+      <c r="C113" s="2">
         <v>4.8062826560804871E-3</v>
       </c>
-      <c r="C113">
+      <c r="D113">
         <v>555</v>
       </c>
-      <c r="D113">
+      <c r="E113">
         <v>-16.001073537790557</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>5</v>
       </c>
       <c r="B114" s="2">
+        <v>1.3668943254789891</v>
+      </c>
+      <c r="C114" s="2">
         <v>4.8095321916973724E-3</v>
       </c>
-      <c r="C114">
+      <c r="D114">
         <v>560</v>
       </c>
-      <c r="D114">
+      <c r="E114">
         <v>-15.865428378724701</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>5</v>
       </c>
       <c r="B115" s="2">
+        <v>1.3556908698157031</v>
+      </c>
+      <c r="C115" s="2">
         <v>4.8127021791814981E-3</v>
       </c>
-      <c r="C115">
+      <c r="D115">
         <v>565</v>
       </c>
-      <c r="D115">
+      <c r="E115">
         <v>-15.73200605483299</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>5</v>
       </c>
       <c r="B116" s="2">
+        <v>1.3446624598054635</v>
+      </c>
+      <c r="C116" s="2">
         <v>4.8157951440224202E-3</v>
       </c>
-      <c r="C116">
+      <c r="D116">
         <v>570</v>
       </c>
-      <c r="D116">
+      <c r="E116">
         <v>-15.600753783416312</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>5</v>
       </c>
       <c r="B117" s="2">
+        <v>1.3338052011081141</v>
+      </c>
+      <c r="C117" s="2">
         <v>4.8188135142892734E-3</v>
       </c>
-      <c r="C117">
+      <c r="D117">
         <v>575</v>
       </c>
-      <c r="D117">
+      <c r="E117">
         <v>-15.471620393742553</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>5</v>
       </c>
       <c r="B118" s="2">
+        <v>1.3231153081398139</v>
+      </c>
+      <c r="C118" s="2">
         <v>4.8217596250089119E-3</v>
       </c>
-      <c r="C118">
+      <c r="D118">
         <v>580</v>
       </c>
-      <c r="D118">
+      <c r="E118">
         <v>-15.344556267853729</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>5</v>
       </c>
       <c r="B119" s="2">
+        <v>1.312589100555934</v>
+      </c>
+      <c r="C119" s="2">
         <v>4.8246357223216095E-3</v>
       </c>
-      <c r="C119">
+      <c r="D119">
         <v>585</v>
       </c>
-      <c r="D119">
+      <c r="E119">
         <v>-15.219513283870612</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>5</v>
       </c>
       <c r="B120" s="2">
+        <v>1.3022229998561521</v>
+      </c>
+      <c r="C120" s="2">
         <v>4.8274439674268251E-3</v>
       </c>
-      <c r="C120">
+      <c r="D120">
         <v>590</v>
       </c>
-      <c r="D120">
+      <c r="E120">
         <v>-15.096444761677711</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>5</v>
       </c>
       <c r="B121" s="2">
+        <v>1.2920135261076982</v>
+      </c>
+      <c r="C121" s="2">
         <v>4.8301864403307191E-3</v>
       </c>
-      <c r="C121">
+      <c r="D121">
         <v>595</v>
       </c>
-      <c r="D121">
+      <c r="E121">
         <v>-14.975305410878008</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>5</v>
       </c>
       <c r="B122" s="2">
+        <v>1.2819572947827693</v>
+      </c>
+      <c r="C122" s="2">
         <v>4.8328651434064712E-3</v>
       </c>
-      <c r="C122">
+      <c r="D122">
         <v>600</v>
       </c>
-      <c r="D122">
+      <c r="E122">
         <v>-14.856051280911808</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>5</v>
       </c>
       <c r="B123" s="2">
+        <v>1.2720510137062446</v>
+      </c>
+      <c r="C123" s="2">
         <v>4.8354820047776942E-3</v>
       </c>
-      <c r="C123">
+      <c r="D123">
         <v>605</v>
       </c>
-      <c r="D123">
+      <c r="E123">
         <v>-14.738639713239829</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>5</v>
       </c>
       <c r="B124" s="2">
+        <v>1.2622914801099003</v>
+      </c>
+      <c r="C124" s="2">
         <v>4.8380388815347439E-3</v>
       </c>
-      <c r="C124">
+      <c r="D124">
         <v>610</v>
       </c>
-      <c r="D124">
+      <c r="E124">
         <v>-14.623029295495192</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>5</v>
       </c>
       <c r="B125" s="2">
+        <v>1.2526755777894314</v>
+      </c>
+      <c r="C125" s="2">
         <v>4.8405375627929908E-3</v>
       </c>
-      <c r="C125">
+      <c r="D125">
         <v>615</v>
       </c>
-      <c r="D125">
+      <c r="E125">
         <v>-14.509179817514061</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>5</v>
       </c>
       <c r="B126" s="2">
+        <v>1.2432002743606914</v>
+      </c>
+      <c r="C126" s="2">
         <v>4.8429797726017298E-3</v>
       </c>
-      <c r="C126">
+      <c r="D126">
         <v>620</v>
       </c>
-      <c r="D126">
+      <c r="E126">
         <v>-14.397052229158962</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>5</v>
       </c>
       <c r="B127" s="2">
+        <v>1.2338626186116461</v>
+      </c>
+      <c r="C127" s="2">
         <v>4.8453671727117656E-3</v>
       </c>
-      <c r="C127">
+      <c r="D127">
         <v>625</v>
       </c>
-      <c r="D127">
+      <c r="E127">
         <v>-14.286608599853135</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>5</v>
       </c>
       <c r="B128" s="2">
+        <v>1.2246597379466582</v>
+      </c>
+      <c r="C128" s="2">
         <v>4.8477013652093318E-3</v>
       </c>
-      <c r="C128">
+      <c r="D128">
         <v>630</v>
       </c>
-      <c r="D128">
+      <c r="E128">
         <v>-14.177812079748289</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>5</v>
       </c>
       <c r="B129" s="2">
+        <v>1.2155888359197977</v>
+      </c>
+      <c r="C129" s="2">
         <v>4.8499838950234828E-3</v>
       </c>
-      <c r="C129">
+      <c r="D129">
         <v>635</v>
       </c>
-      <c r="D129">
+      <c r="E129">
         <v>-14.07062686245197</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>5</v>
       </c>
       <c r="B130" s="2">
+        <v>1.2066471898540008</v>
+      </c>
+      <c r="C130" s="2">
         <v>4.8522162523137241E-3</v>
       </c>
-      <c r="C130">
+      <c r="D130">
         <v>640</v>
       </c>
-      <c r="D130">
+      <c r="E130">
         <v>-13.965018149244369</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>5</v>
       </c>
       <c r="B131" s="2">
+        <v>1.1978321485429824</v>
+      </c>
+      <c r="C131" s="2">
         <v>4.8543998747442411E-3</v>
       </c>
-      <c r="C131">
+      <c r="D131">
         <v>645</v>
       </c>
-      <c r="D131">
+      <c r="E131">
         <v>-13.860952114717817</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>5</v>
       </c>
       <c r="B132" s="2">
+        <v>1.1891411300329078</v>
+      </c>
+      <c r="C132" s="2">
         <v>4.8565361496507014E-3</v>
       </c>
-      <c r="C132">
+      <c r="D132">
         <v>650</v>
       </c>
-      <c r="D132">
+      <c r="E132">
         <v>-13.758395873775521</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>5</v>
       </c>
       <c r="B133" s="2">
+        <v>1.1805716194809419</v>
+      </c>
+      <c r="C133" s="2">
         <v>4.8586264161052904E-3</v>
       </c>
-      <c r="C133">
+      <c r="D133">
         <v>655</v>
       </c>
-      <c r="D133">
+      <c r="E133">
         <v>-13.657317449929096</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>5</v>
       </c>
       <c r="B134" s="2">
+        <v>1.1721211670878788</v>
+      </c>
+      <c r="C134" s="2">
         <v>4.8606719668852945E-3</v>
       </c>
-      <c r="C134">
+      <c r="D134">
         <v>660</v>
       </c>
-      <c r="D134">
+      <c r="E134">
         <v>-13.557685744837523</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>5</v>
       </c>
       <c r="B135" s="2">
+        <v>1.1637873861021466</v>
+      </c>
+      <c r="C135" s="2">
         <v>4.8626740503502327E-3</v>
       </c>
-      <c r="C135">
+      <c r="D135">
         <v>665</v>
       </c>
-      <c r="D135">
+      <c r="E135">
         <v>-13.459470509032789</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>5</v>
       </c>
       <c r="B136" s="2">
+        <v>1.1555679508925958</v>
+      </c>
+      <c r="C136" s="2">
         <v>4.8646338722323065E-3</v>
       </c>
-      <c r="C136">
+      <c r="D136">
         <v>670</v>
       </c>
-      <c r="D136">
+      <c r="E136">
         <v>-13.362642313780198</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>5</v>
       </c>
       <c r="B137" s="2">
+        <v>1.1474605950875452</v>
+      </c>
+      <c r="C137" s="2">
         <v>4.8665525973445858E-3</v>
       </c>
-      <c r="C137">
+      <c r="D137">
         <v>675</v>
       </c>
-      <c r="D137">
+      <c r="E137">
         <v>-13.267172524023815</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>5</v>
       </c>
       <c r="B138" s="2">
+        <v>1.139463109777666</v>
+      </c>
+      <c r="C138" s="2">
         <v>4.868431351211169E-3</v>
       </c>
-      <c r="C138">
+      <c r="D138">
         <v>680</v>
       </c>
-      <c r="D138">
+      <c r="E138">
         <v>-13.173033272369892</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>5</v>
       </c>
       <c r="B139" s="2">
+        <v>1.1315733417803655</v>
+      </c>
+      <c r="C139" s="2">
         <v>4.8702712216232898E-3</v>
       </c>
-      <c r="C139">
+      <c r="D139">
         <v>685</v>
       </c>
-      <c r="D139">
+      <c r="E139">
         <v>-13.080197434063317</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>5</v>
       </c>
       <c r="B140" s="2">
+        <v>1.1237891919634178</v>
+      </c>
+      <c r="C140" s="2">
         <v>4.8720732601251196E-3</v>
       </c>
-      <c r="C140">
+      <c r="D140">
         <v>690</v>
       </c>
-      <c r="D140">
+      <c r="E140">
         <v>-12.988638602914387</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>5</v>
       </c>
       <c r="B141" s="2">
+        <v>1.1161086136256657</v>
+      </c>
+      <c r="C141" s="2">
         <v>4.8738384834328052E-3</v>
       </c>
-      <c r="C141">
+      <c r="D141">
         <v>695</v>
       </c>
-      <c r="D141">
+      <c r="E141">
         <v>-12.898331068135088</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>5</v>
       </c>
       <c r="B142" s="2">
+        <v>1.1085296109327052</v>
+      </c>
+      <c r="C142" s="2">
         <v>4.8755678747901135E-3</v>
       </c>
-      <c r="C142">
+      <c r="D142">
         <v>700</v>
       </c>
-      <c r="D142">
+      <c r="E142">
         <v>-12.809249792046058</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>5</v>
       </c>
       <c r="B143" s="2">
+        <v>1.1010502374055364</v>
+      </c>
+      <c r="C143" s="2">
         <v>4.8772623852638081E-3</v>
       </c>
-      <c r="C143">
+      <c r="D143">
         <v>705</v>
       </c>
-      <c r="D143">
+      <c r="E143">
         <v>-12.721370388617293</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>5</v>
       </c>
       <c r="B144" s="2">
+        <v>1.09366859446024</v>
+      </c>
+      <c r="C144" s="2">
         <v>4.8789229349817942E-3</v>
       </c>
-      <c r="C144">
+      <c r="D144">
         <v>710</v>
       </c>
-      <c r="D144">
+      <c r="E144">
         <v>-12.63466910280728</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>5</v>
       </c>
       <c r="B145" s="2">
+        <v>1.0863828299968115</v>
+      </c>
+      <c r="C145" s="2">
         <v>4.880550414316823E-3</v>
       </c>
-      <c r="C145">
+      <c r="D145">
         <v>715</v>
       </c>
-      <c r="D145">
+      <c r="E145">
         <v>-12.549122790666928</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>5</v>
       </c>
       <c r="B146" s="2">
+        <v>1.0791911370353542</v>
+      </c>
+      <c r="C146" s="2">
         <v>4.882145685018457E-3</v>
       </c>
-      <c r="C146">
+      <c r="D146">
         <v>720</v>
       </c>
-      <c r="D146">
+      <c r="E146">
         <v>-12.464708900176291</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>5</v>
       </c>
       <c r="B147" s="2">
+        <v>1.0720917523978994</v>
+      </c>
+      <c r="C147" s="2">
         <v>4.8837095812957997E-3</v>
       </c>
-      <c r="C147">
+      <c r="D147">
         <v>725</v>
       </c>
-      <c r="D147">
+      <c r="E147">
         <v>-12.381405452783447</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>5</v>
       </c>
       <c r="B148" s="2">
+        <v>1.0650829554341925</v>
+      </c>
+      <c r="C148" s="2">
         <v>4.8852429108534167E-3</v>
       </c>
-      <c r="C148">
+      <c r="D148">
         <v>730</v>
       </c>
-      <c r="D148">
+      <c r="E148">
         <v>-12.299191025616434</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>5</v>
       </c>
       <c r="B149" s="2">
+        <v>1.0581630667898356</v>
+      </c>
+      <c r="C149" s="2">
         <v>4.8867464558826797E-3</v>
       </c>
-      <c r="C149">
+      <c r="D149">
         <v>735</v>
       </c>
-      <c r="D149">
+      <c r="E149">
         <v>-12.218044734340392</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>5</v>
       </c>
       <c r="B150" s="2">
+        <v>1.0513304472152476</v>
+      </c>
+      <c r="C150" s="2">
         <v>4.8882209740107067E-3</v>
       </c>
-      <c r="C150">
+      <c r="D150">
         <v>740</v>
       </c>
-      <c r="D150">
+      <c r="E150">
         <v>-12.137946216633315</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>5</v>
       </c>
       <c r="B151" s="2">
+        <v>1.0445834964139633</v>
+      </c>
+      <c r="C151" s="2">
         <v>4.8896671992089179E-3</v>
       </c>
-      <c r="C151">
+      <c r="D151">
         <v>745</v>
       </c>
-      <c r="D151">
+      <c r="E151">
         <v>-12.058875616255193</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>5</v>
       </c>
       <c r="B152" s="2">
+        <v>1.0379206519288324</v>
+      </c>
+      <c r="C152" s="2">
         <v>4.8910858426631223E-3</v>
       </c>
-      <c r="C152">
+      <c r="D152">
         <v>750</v>
       </c>
-      <c r="D152">
+      <c r="E152">
         <v>-11.980813567686223</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>5</v>
       </c>
       <c r="B153" s="2">
+        <v>1.0313403880647596</v>
+      </c>
+      <c r="C153" s="2">
         <v>4.8924775936069892E-3</v>
       </c>
-      <c r="C153">
+      <c r="D153">
         <v>755</v>
       </c>
-      <c r="D153">
+      <c r="E153">
         <v>-11.903741181311082</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>5</v>
       </c>
       <c r="B154" s="2">
+        <v>1.0248412148466528</v>
+      </c>
+      <c r="C154" s="2">
         <v>4.8938431201205907E-3</v>
       </c>
-      <c r="C154">
+      <c r="D154">
         <v>760</v>
       </c>
-      <c r="D154">
+      <c r="E154">
         <v>-11.827640029127174</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>5</v>
       </c>
       <c r="B155" s="2">
+        <v>1.018421677011319</v>
+      </c>
+      <c r="C155" s="2">
         <v>4.895183069895696E-3</v>
       </c>
-      <c r="C155">
+      <c r="D155">
         <v>765</v>
       </c>
-      <c r="D155">
+      <c r="E155">
         <v>-11.752492130955805</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>5</v>
       </c>
       <c r="B156" s="2">
+        <v>1.0120803530320786</v>
+      </c>
+      <c r="C156" s="2">
         <v>4.8964980709693398E-3</v>
       </c>
-      <c r="C156">
+      <c r="D156">
         <v>770</v>
       </c>
-      <c r="D156">
+      <c r="E156">
         <v>-11.678279941136104</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>5</v>
       </c>
       <c r="B157" s="2">
+        <v>1.0058158541749282</v>
+      </c>
+      <c r="C157" s="2">
         <v>4.8977887324271512E-3</v>
       </c>
-      <c r="C157">
+      <c r="D157">
         <v>775</v>
       </c>
-      <c r="D157">
+      <c r="E157">
         <v>-11.604986335682554</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>5</v>
       </c>
       <c r="B158" s="2">
+        <v>0.99962682358512001</v>
+      </c>
+      <c r="C158" s="2">
         <v>4.8990556450778473E-3</v>
       </c>
-      <c r="C158">
+      <c r="D158">
         <v>780</v>
       </c>
-      <c r="D158">
+      <c r="E158">
         <v>-11.532594599887657</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>5</v>
       </c>
       <c r="B159" s="2">
+        <v>0.99351193540306759</v>
+      </c>
+      <c r="C159" s="2">
         <v>4.9002993821002051E-3</v>
       </c>
-      <c r="C159">
+      <c r="D159">
         <v>785</v>
       </c>
-      <c r="D159">
+      <c r="E159">
         <v>-11.461088416352226</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>5</v>
       </c>
       <c r="B160" s="2">
+        <v>0.98746989390854067</v>
+      </c>
+      <c r="C160" s="2">
         <v>4.9015204996637786E-3</v>
       </c>
-      <c r="C160">
+      <c r="D160">
         <v>790</v>
       </c>
-      <c r="D160">
+      <c r="E160">
         <v>-11.390451853426505</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>5</v>
       </c>
       <c r="B161" s="2">
+        <v>0.98149943269213169</v>
+      </c>
+      <c r="C161" s="2">
         <v>4.9027195375245585E-3</v>
       </c>
-      <c r="C161">
+      <c r="D161">
         <v>795</v>
       </c>
-      <c r="D161">
+      <c r="E161">
         <v>-11.320669354045997</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>5</v>
       </c>
       <c r="B162" s="2">
+        <v>0.97559931385303666</v>
+      </c>
+      <c r="C162" s="2">
         <v>4.9038970195967087E-3</v>
       </c>
-      <c r="C162">
+      <c r="D162">
         <v>800</v>
       </c>
-      <c r="D162">
+      <c r="E162">
         <v>-11.251725724946706</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>5</v>
       </c>
       <c r="B163" s="2">
+        <v>0.96976832722221518</v>
+      </c>
+      <c r="C163" s="2">
         <v>4.9050534545014516E-3</v>
       </c>
-      <c r="C163">
+      <c r="D163">
         <v>805</v>
       </c>
-      <c r="D163">
+      <c r="E163">
         <v>-11.183606126245074</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>5</v>
       </c>
       <c r="B164" s="2">
+        <v>0.96400528961003351</v>
+      </c>
+      <c r="C164" s="2">
         <v>4.9061893360941421E-3</v>
       </c>
-      <c r="C164">
+      <c r="D164">
         <v>810</v>
       </c>
-      <c r="D164">
+      <c r="E164">
         <v>-11.116296061368519</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>5</v>
       </c>
       <c r="B165" s="2">
+        <v>0.9583090440775317</v>
+      </c>
+      <c r="C165" s="2">
         <v>4.9073051439704881E-3</v>
       </c>
-      <c r="C165">
+      <c r="D165">
         <v>815</v>
       </c>
-      <c r="D165">
+      <c r="E165">
         <v>-11.049781367323147</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>5</v>
       </c>
       <c r="B166" s="2">
+        <v>0.95267845923048755</v>
+      </c>
+      <c r="C166" s="2">
         <v>4.9084013439528581E-3</v>
       </c>
-      <c r="C166">
+      <c r="D166">
         <v>820</v>
       </c>
-      <c r="D166">
+      <c r="E166">
         <v>-10.984048205285776</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>5</v>
       </c>
       <c r="B167" s="2">
+        <v>0.94711242853547506</v>
+      </c>
+      <c r="C167" s="2">
         <v>4.90947838855755E-3</v>
       </c>
-      <c r="C167">
+      <c r="D167">
         <v>825</v>
       </c>
-      <c r="D167">
+      <c r="E167">
         <v>-10.919083051507858</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>5</v>
       </c>
       <c r="B168" s="2">
+        <v>0.9416098696571551</v>
+      </c>
+      <c r="C168" s="2">
         <v>4.9105367174438518E-3</v>
       </c>
-      <c r="C168">
+      <c r="D168">
         <v>830</v>
       </c>
-      <c r="D168">
+      <c r="E168">
         <v>-10.854872688519606</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>5</v>
       </c>
       <c r="B169" s="2">
+        <v>0.93616972381605945</v>
+      </c>
+      <c r="C169" s="2">
         <v>4.9115767578457089E-3</v>
       </c>
-      <c r="C169">
+      <c r="D169">
         <v>835</v>
       </c>
-      <c r="D169">
+      <c r="E169">
         <v>-10.791404196622912</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>5</v>
       </c>
       <c r="B170" s="2">
+        <v>0.93079095516615584</v>
+      </c>
+      <c r="C170" s="2">
         <v>4.9125989249867406E-3</v>
       </c>
-      <c r="C170">
+      <c r="D170">
         <v>840</v>
       </c>
-      <c r="D170">
+      <c r="E170">
         <v>-10.728664945662263</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>5</v>
       </c>
       <c r="B171" s="2">
+        <v>0.92547255019151375</v>
+      </c>
+      <c r="C171" s="2">
         <v>4.9136036224793327E-3</v>
       </c>
-      <c r="C171">
+      <c r="D171">
         <v>845</v>
       </c>
-      <c r="D171">
+      <c r="E171">
         <v>-10.666642587063317</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>5</v>
       </c>
       <c r="B172" s="2">
+        <v>0.92021351712140975</v>
+      </c>
+      <c r="C172" s="2">
         <v>4.9145912427084968E-3</v>
       </c>
-      <c r="C172">
+      <c r="D172">
         <v>850</v>
       </c>
-      <c r="D172">
+      <c r="E172">
         <v>-10.605325046129094</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>5</v>
       </c>
       <c r="B173" s="2">
+        <v>0.91501288536324232</v>
+      </c>
+      <c r="C173" s="2">
         <v>4.9155621672011462E-3</v>
       </c>
-      <c r="C173">
+      <c r="D173">
         <v>855</v>
       </c>
-      <c r="D173">
+      <c r="E173">
         <v>-10.54470051458434</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>5</v>
       </c>
       <c r="B174" s="2">
+        <v>0.90986970495264707</v>
+      </c>
+      <c r="C174" s="2">
         <v>4.9165167669814151E-3</v>
       </c>
-      <c r="C174">
+      <c r="D174">
         <v>860</v>
       </c>
-      <c r="D174">
+      <c r="E174">
         <v>-10.484757443358902</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>5</v>
       </c>
       <c r="B175" s="2">
+        <v>0.90478304602021842</v>
+      </c>
+      <c r="C175" s="2">
         <v>4.9174554029126055E-3</v>
       </c>
-      <c r="C175">
+      <c r="D175">
         <v>865</v>
       </c>
-      <c r="D175">
+      <c r="E175">
         <v>-10.425484535601278</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>5</v>
       </c>
       <c r="B176" s="2">
+        <v>0.89975199827428654</v>
+      </c>
+      <c r="C176" s="2">
         <v>4.9183784260263489E-3</v>
       </c>
-      <c r="C176">
+      <c r="D176">
         <v>870</v>
       </c>
-      <c r="D176">
+      <c r="E176">
         <v>-10.366870739914079</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>5</v>
       </c>
       <c r="B177" s="2">
+        <v>0.89477567049919138</v>
+      </c>
+      <c r="C177" s="2">
         <v>4.9192861778394967E-3</v>
       </c>
-      <c r="C177">
+      <c r="D177">
         <v>875</v>
       </c>
-      <c r="D177">
+      <c r="E177">
         <v>-10.308905243803196</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>5</v>
       </c>
       <c r="B178" s="2">
+        <v>0.88985319006853936</v>
+      </c>
+      <c r="C178" s="2">
         <v>4.9201789906592672E-3</v>
       </c>
-      <c r="C178">
+      <c r="D178">
         <v>880</v>
       </c>
-      <c r="D178">
+      <c r="E178">
         <v>-10.251577467333055</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>5</v>
       </c>
       <c r="B179" s="2">
+        <v>0.88498370247293701</v>
+      </c>
+      <c r="C179" s="2">
         <v>4.921057187877143E-3</v>
       </c>
-      <c r="C179">
+      <c r="D179">
         <v>885</v>
       </c>
-      <c r="D179">
+      <c r="E179">
         <v>-10.194877056980458</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>5</v>
       </c>
       <c r="B180" s="2">
+        <v>0.88016637086171112</v>
+      </c>
+      <c r="C180" s="2">
         <v>4.9219210842519736E-3</v>
       </c>
-      <c r="C180">
+      <c r="D180">
         <v>890</v>
       </c>
-      <c r="D180">
+      <c r="E180">
         <v>-10.138793879679953</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>5</v>
       </c>
       <c r="B181" s="2">
+        <v>0.8754003755981542</v>
+      </c>
+      <c r="C181" s="2">
         <v>4.922770986182743E-3</v>
       </c>
-      <c r="C181">
+      <c r="D181">
         <v>895</v>
       </c>
-      <c r="D181">
+      <c r="E181">
         <v>-10.083318017053848</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>5</v>
       </c>
       <c r="B182" s="2">
+        <v>0.87068491382784052</v>
+      </c>
+      <c r="C182" s="2">
         <v>4.923607191971411E-3</v>
       </c>
-      <c r="C182">
+      <c r="D182">
         <v>900</v>
       </c>
-      <c r="D182">
+      <c r="E182">
         <v>-10.028439759820365</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>5</v>
       </c>
       <c r="B183" s="2">
+        <v>0.86601919905958002</v>
+      </c>
+      <c r="C183" s="2">
         <v>4.9244299920762607E-3</v>
       </c>
-      <c r="C183">
+      <c r="D183">
         <v>905</v>
       </c>
-      <c r="D183">
+      <c r="E183">
         <v>-9.9741496023735614</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>5</v>
       </c>
       <c r="B184" s="2">
+        <v>0.86140246075858951</v>
+      </c>
+      <c r="C184" s="2">
         <v>4.9252396693561058E-3</v>
       </c>
-      <c r="C184">
+      <c r="D184">
         <v>910</v>
       </c>
-      <c r="D184">
+      <c r="E184">
         <v>-9.9204382375290336</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>5</v>
       </c>
       <c r="B185" s="2">
+        <v>0.85683394395148371</v>
+      </c>
+      <c r="C185" s="2">
         <v>4.9260364993057599E-3</v>
       </c>
-      <c r="C185">
+      <c r="D185">
         <v>915</v>
       </c>
-      <c r="D185">
+      <c r="E185">
         <v>-9.867296551429579</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>5</v>
       </c>
       <c r="B186" s="2">
+        <v>0.85231290884269084</v>
+      </c>
+      <c r="C186" s="2">
         <v>4.926820750283098E-3</v>
       </c>
-      <c r="C186">
+      <c r="D186">
         <v>920</v>
       </c>
-      <c r="D186">
+      <c r="E186">
         <v>-9.8147156186051951</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>5</v>
       </c>
       <c r="B187" s="2">
+        <v>0.84783863044192453</v>
+      </c>
+      <c r="C187" s="2">
         <v>4.9275926837280661E-3</v>
       </c>
-      <c r="C187">
+      <c r="D187">
         <v>925</v>
       </c>
-      <c r="D187">
+      <c r="E187">
         <v>-9.762686697182108</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>5</v>
       </c>
       <c r="B188" s="2">
+        <v>0.84341039820234609</v>
+      </c>
+      <c r="C188" s="2">
         <v>4.9283525543739421E-3</v>
       </c>
-      <c r="C188">
+      <c r="D188">
         <v>930</v>
       </c>
-      <c r="D188">
+      <c r="E188">
         <v>-9.7112012242356265</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>5</v>
       </c>
       <c r="B189" s="2">
+        <v>0.83902751566907363</v>
+      </c>
+      <c r="C189" s="2">
         <v>4.9291006104511788E-3</v>
       </c>
-      <c r="C189">
+      <c r="D189">
         <v>935</v>
       </c>
-      <c r="D189">
+      <c r="E189">
         <v>-9.6602508112819052</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>5</v>
       </c>
       <c r="B190" s="2">
+        <v>0.83468930013770082</v>
+      </c>
+      <c r="C190" s="2">
         <v>4.9298370938841004E-3</v>
       </c>
-      <c r="C190">
+      <c r="D190">
         <v>940</v>
       </c>
-      <c r="D190">
+      <c r="E190">
         <v>-9.6098272399038507</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>5</v>
       </c>
       <c r="B191" s="2">
+        <v>0.83039508232250026</v>
+      </c>
+      <c r="C191" s="2">
         <v>4.9305622404807554E-3</v>
       </c>
-      <c r="C191">
+      <c r="D191">
         <v>945</v>
       </c>
-      <c r="D191">
+      <c r="E191">
         <v>-9.5599224575065307</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>5</v>
       </c>
       <c r="B192" s="2">
+        <v>0.82614420603400385</v>
+      </c>
+      <c r="C192" s="2">
         <v>4.9312762801161777E-3</v>
       </c>
-      <c r="C192">
+      <c r="D192">
         <v>950</v>
       </c>
-      <c r="D192">
+      <c r="E192">
         <v>-9.5105285731977904</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>5</v>
       </c>
       <c r="B193" s="2">
+        <v>0.82193602786565623</v>
+      </c>
+      <c r="C193" s="2">
         <v>4.9319794369093251E-3</v>
       </c>
-      <c r="C193">
+      <c r="D193">
         <v>955</v>
       </c>
-      <c r="D193">
+      <c r="E193">
         <v>-9.4616378537897425</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>5</v>
       </c>
       <c r="B194" s="2">
+        <v>0.8177699168892526</v>
+      </c>
+      <c r="C194" s="2">
         <v>4.9326719293939416E-3</v>
       </c>
-      <c r="C194">
+      <c r="D194">
         <v>960</v>
       </c>
-      <c r="D194">
+      <c r="E194">
         <v>-9.41324271991712</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>5</v>
       </c>
       <c r="B195" s="2">
+        <v>0.81364525435887913</v>
+      </c>
+      <c r="C195" s="2">
         <v>4.9333539706835627E-3</v>
       </c>
-      <c r="C195">
+      <c r="D195">
         <v>965</v>
       </c>
-      <c r="D195">
+      <c r="E195">
         <v>-9.3653357422685168</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>5</v>
       </c>
       <c r="B196" s="2">
+        <v>0.80956143342309228</v>
+      </c>
+      <c r="C196" s="2">
         <v>4.9340257686309209E-3</v>
       </c>
-      <c r="C196">
+      <c r="D196">
         <v>970</v>
       </c>
-      <c r="D196">
+      <c r="E196">
         <v>-9.3179096379267996</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>5</v>
       </c>
       <c r="B197" s="2">
+        <v>0.80551785884506644</v>
+      </c>
+      <c r="C197" s="2">
         <v>4.93468752598193E-3</v>
       </c>
-      <c r="C197">
+      <c r="D197">
         <v>975</v>
       </c>
-      <c r="D197">
+      <c r="E197">
         <v>-9.2709572668150351</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>5</v>
       </c>
       <c r="B198" s="2">
+        <v>0.80151394673047049</v>
+      </c>
+      <c r="C198" s="2">
         <v>4.9353394405244853E-3</v>
       </c>
-      <c r="C198">
+      <c r="D198">
         <v>980</v>
       </c>
-      <c r="D198">
+      <c r="E198">
         <v>-9.2244716282444106</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>5</v>
       </c>
       <c r="B199" s="2">
+        <v>0.79754912426281988</v>
+      </c>
+      <c r="C199" s="2">
         <v>4.935981705232264E-3</v>
       </c>
-      <c r="C199">
+      <c r="D199">
         <v>985</v>
       </c>
-      <c r="D199">
+      <c r="E199">
         <v>-9.1784458575608436</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>5</v>
       </c>
       <c r="B200" s="2">
+        <v>0.79362282944607798</v>
+      </c>
+      <c r="C200" s="2">
         <v>4.9366145084037095E-3</v>
       </c>
-      <c r="C200">
+      <c r="D200">
         <v>990</v>
       </c>
-      <c r="D200">
+      <c r="E200">
         <v>-9.1328732228869747</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>5</v>
       </c>
       <c r="B201" s="2">
+        <v>0.78973451085427904</v>
+      </c>
+      <c r="C201" s="2">
         <v>4.9372380337964015E-3</v>
       </c>
-      <c r="C201">
+      <c r="D201">
         <v>995</v>
       </c>
-      <c r="D201">
+      <c r="E201">
         <v>-9.0877471219564896</v>
       </c>
     </row>

</xml_diff>